<commit_message>
Improving field descriptions on excel template
</commit_message>
<xml_diff>
--- a/Excel Template.xlsx
+++ b/Excel Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://veracode-my.sharepoint.com/personal/rpereira_veracode_com/Documents/Projects/plugins/Veracode-Bulk-Application-Creator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_6C5D155443060114056EE7543FCFA25781696894" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{78E1B274-BF18-4DA4-AB8E-2F4630A9EE7C}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="11_6C5D155443060114056EE7543FCFA25781696894" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A717AFDD-3189-4688-A9C5-0494FE0B72EA}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,14 +20,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>This template can be used to bulk import applications into the Veracode platform by using the plugin at https://github.com/cadonuno/Veracode-Bulk-Application-Creator. Above each field name, there's a description of the allowed values. After execution, a new column will be added with the status of each application</t>
   </si>
   <si>
-    <t>Case-sensitive policy name</t>
-  </si>
-  <si>
     <t>Allows for the values specified here: https://docs.veracode.com/r/r_updateapp</t>
   </si>
   <si>
@@ -43,12 +40,6 @@
     <t>Custom fields can be renamed, in that case, you need to put their real name here</t>
   </si>
   <si>
-    <t>Application Name</t>
-  </si>
-  <si>
-    <t>Business Criticality</t>
-  </si>
-  <si>
     <t>Policy</t>
   </si>
   <si>
@@ -161,13 +152,25 @@
   </si>
   <si>
     <t>Custom 25</t>
+  </si>
+  <si>
+    <t>Application Name*</t>
+  </si>
+  <si>
+    <t>Business Criticality*</t>
+  </si>
+  <si>
+    <t>Case-sensitive policy name (defaults to the one assigned to the Business Criticality)</t>
+  </si>
+  <si>
+    <t>Comma-delimited list of teams</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -177,6 +180,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -204,12 +215,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -225,6 +239,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -527,13 +545,13 @@
   <dimension ref="A1:AN2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="34.81640625" customWidth="1"/>
-    <col min="2" max="2" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.453125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30.453125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="30.453125" customWidth="1"/>
     <col min="5" max="5" width="33.7265625" bestFit="1" customWidth="1"/>
@@ -557,148 +575,151 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="M1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="P1" s="3" t="s">
         <v>5</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="O2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="P2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="Q2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="R2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="S2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="T2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="U2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="S2" s="2" t="s">
+      <c r="V2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="T2" s="2" t="s">
+      <c r="W2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="U2" s="2" t="s">
+      <c r="X2" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="V2" s="2" t="s">
+      <c r="Y2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="W2" s="2" t="s">
+      <c r="Z2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="X2" s="2" t="s">
+      <c r="AA2" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="Y2" s="2" t="s">
+      <c r="AB2" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="Z2" s="2" t="s">
+      <c r="AC2" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AA2" s="2" t="s">
+      <c r="AD2" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="AB2" s="2" t="s">
+      <c r="AE2" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="AC2" s="2" t="s">
+      <c r="AF2" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="AD2" s="2" t="s">
+      <c r="AG2" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="AE2" s="2" t="s">
+      <c r="AH2" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="AF2" s="2" t="s">
+      <c r="AI2" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="AG2" s="2" t="s">
+      <c r="AJ2" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="AH2" s="2" t="s">
+      <c r="AK2" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AI2" s="2" t="s">
+      <c r="AL2" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="AJ2" s="2" t="s">
+      <c r="AM2" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="AK2" s="2" t="s">
+      <c r="AN2" s="2" t="s">
         <v>43</v>
-      </c>
-      <c r="AL2" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="AM2" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="AN2" s="2" t="s">
-        <v>46</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixing issue with excel template
</commit_message>
<xml_diff>
--- a/Excel Template.xlsx
+++ b/Excel Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://veracode-my.sharepoint.com/personal/rpereira_veracode_com/Documents/Projects/plugins/Veracode-Bulk-Application-Creator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="11_6C5D155443060114056EE7543FCFA25781696894" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A717AFDD-3189-4688-A9C5-0494FE0B72EA}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="11_6C5D155443060114056EE7543FCFA25781696894" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6E399F53-8C97-4A9B-920B-A893EFC44C40}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
   <si>
     <t>This template can be used to bulk import applications into the Veracode platform by using the plugin at https://github.com/cadonuno/Veracode-Bulk-Application-Creator. Above each field name, there's a description of the allowed values. After execution, a new column will be added with the status of each application</t>
   </si>
@@ -154,16 +154,19 @@
     <t>Custom 25</t>
   </si>
   <si>
-    <t>Application Name*</t>
-  </si>
-  <si>
-    <t>Business Criticality*</t>
-  </si>
-  <si>
     <t>Case-sensitive policy name (defaults to the one assigned to the Business Criticality)</t>
   </si>
   <si>
     <t>Comma-delimited list of teams</t>
+  </si>
+  <si>
+    <t>Business Criticality</t>
+  </si>
+  <si>
+    <t>Mandatory*</t>
+  </si>
+  <si>
+    <t>Application Name</t>
   </si>
 </sst>
 </file>
@@ -215,13 +218,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -545,7 +551,7 @@
   <dimension ref="A1:AN2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -574,8 +580,11 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="4" t="s">
+        <v>47</v>
+      </c>
       <c r="C1" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -590,7 +599,7 @@
         <v>4</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="P1" s="3" t="s">
         <v>5</v>
@@ -598,10 +607,10 @@
     </row>
     <row r="2" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>6</v>

</xml_diff>